<commit_message>
updated client to couple with backend
</commit_message>
<xml_diff>
--- a/uploads/books.xlsx
+++ b/uploads/books.xlsx
@@ -4,30 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9950"/>
+    <workbookView windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="books" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Title</t>
   </si>
@@ -129,12 +116,21 @@
   </si>
   <si>
     <t>CRC</t>
+  </si>
+  <si>
+    <t>How to Think Like Sherlock Holmes</t>
+  </si>
+  <si>
+    <t>Konnikova, Maria</t>
+  </si>
+  <si>
+    <t>psychology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -1281,17 +1277,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="19.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="38.6363636363636" customWidth="1"/>
-    <col min="3" max="3" width="16.4545454545455" customWidth="1"/>
+    <col min="1" max="1" width="27.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="23.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="29.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1432,6 +1429,20 @@
       </c>
       <c r="D10" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>